<commit_message>
Remove bugs factor ggtext and add parameters to functions
</commit_message>
<xml_diff>
--- a/R/data/df_persona_per_group.xlsx
+++ b/R/data/df_persona_per_group.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE15"/>
+  <dimension ref="A1:AE18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D2">
-        <v>915</v>
+        <v>1272</v>
       </c>
       <c r="E2">
-        <v>0.5669999999999999</v>
+        <v>0.351</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -551,7 +551,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -598,31 +598,31 @@
         <v>20</v>
       </c>
       <c r="S2">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="T2">
-        <v>32.4</v>
+        <v>44.5</v>
       </c>
       <c r="U2">
+        <v>6.6</v>
+      </c>
+      <c r="V2">
+        <v>6.6</v>
+      </c>
+      <c r="W2">
         <v>6.4</v>
       </c>
-      <c r="V2">
-        <v>6.4</v>
-      </c>
-      <c r="W2">
+      <c r="X2">
+        <v>6.1</v>
+      </c>
+      <c r="Y2">
+        <v>7.5</v>
+      </c>
+      <c r="Z2">
         <v>5.9</v>
       </c>
-      <c r="X2">
-        <v>6.3</v>
-      </c>
-      <c r="Y2">
-        <v>7</v>
-      </c>
-      <c r="Z2">
-        <v>6.2</v>
-      </c>
       <c r="AA2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
         <v>0</v>
@@ -631,7 +631,7 @@
         <v>0</v>
       </c>
       <c r="AD2">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="3">
@@ -646,13 +646,13 @@
         </is>
       </c>
       <c r="C3">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D3">
-        <v>698</v>
+        <v>2352</v>
       </c>
       <c r="E3">
-        <v>0.433</v>
+        <v>0.649</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -671,7 +671,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>EM&amp;CM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -681,12 +681,12 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -718,31 +718,31 @@
         <v>19</v>
       </c>
       <c r="S3">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="T3">
-        <v>33.4</v>
+        <v>44.5</v>
       </c>
       <c r="U3">
+        <v>6.6</v>
+      </c>
+      <c r="V3">
+        <v>6.6</v>
+      </c>
+      <c r="W3">
         <v>6.4</v>
       </c>
-      <c r="V3">
-        <v>6.4</v>
-      </c>
-      <c r="W3">
+      <c r="X3">
+        <v>6.1</v>
+      </c>
+      <c r="Y3">
+        <v>7.5</v>
+      </c>
+      <c r="Z3">
         <v>5.9</v>
       </c>
-      <c r="X3">
-        <v>6.3</v>
-      </c>
-      <c r="Y3">
-        <v>7</v>
-      </c>
-      <c r="Z3">
-        <v>6.2</v>
-      </c>
       <c r="AA3">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB3">
         <v>0</v>
@@ -766,17 +766,17 @@
         </is>
       </c>
       <c r="C4">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D4">
-        <v>756</v>
+        <v>1739</v>
       </c>
       <c r="E4">
-        <v>0.469</v>
+        <v>0.48</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>MedV</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -801,12 +801,12 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -835,34 +835,34 @@
         </is>
       </c>
       <c r="R4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S4">
-        <v>137.5</v>
+        <v>150</v>
       </c>
       <c r="T4">
-        <v>34.2</v>
+        <v>44.5</v>
       </c>
       <c r="U4">
+        <v>6.6</v>
+      </c>
+      <c r="V4">
+        <v>6.6</v>
+      </c>
+      <c r="W4">
         <v>6.4</v>
       </c>
-      <c r="V4">
-        <v>6.4</v>
-      </c>
-      <c r="W4">
+      <c r="X4">
+        <v>6.1</v>
+      </c>
+      <c r="Y4">
+        <v>7.5</v>
+      </c>
+      <c r="Z4">
         <v>5.9</v>
       </c>
-      <c r="X4">
-        <v>6.3</v>
-      </c>
-      <c r="Y4">
-        <v>7</v>
-      </c>
-      <c r="Z4">
-        <v>6.2</v>
-      </c>
       <c r="AA4">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -871,7 +871,7 @@
         <v>0</v>
       </c>
       <c r="AD4">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="5">
@@ -886,13 +886,13 @@
         </is>
       </c>
       <c r="C5">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D5">
-        <v>176</v>
+        <v>780</v>
       </c>
       <c r="E5">
-        <v>0.109</v>
+        <v>0.215</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -906,17 +906,17 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>MedV</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -958,31 +958,31 @@
         <v>20</v>
       </c>
       <c r="S5">
-        <v>134.5</v>
+        <v>139</v>
       </c>
       <c r="T5">
-        <v>34.7</v>
+        <v>44.5</v>
       </c>
       <c r="U5">
+        <v>6.6</v>
+      </c>
+      <c r="V5">
+        <v>6.6</v>
+      </c>
+      <c r="W5">
         <v>6.4</v>
       </c>
-      <c r="V5">
-        <v>6.4</v>
-      </c>
-      <c r="W5">
+      <c r="X5">
+        <v>6.1</v>
+      </c>
+      <c r="Y5">
+        <v>7.5</v>
+      </c>
+      <c r="Z5">
         <v>5.9</v>
       </c>
-      <c r="X5">
-        <v>6.3</v>
-      </c>
-      <c r="Y5">
-        <v>7</v>
-      </c>
-      <c r="Z5">
-        <v>6.2</v>
-      </c>
       <c r="AA5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB5">
         <v>0</v>
@@ -1006,17 +1006,17 @@
         </is>
       </c>
       <c r="C6">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D6">
-        <v>202</v>
+        <v>259</v>
       </c>
       <c r="E6">
-        <v>0.125</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -1026,37 +1026,37 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>EM&amp;CM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -1078,28 +1078,28 @@
         <v>21</v>
       </c>
       <c r="S6">
-        <v>128.5</v>
+        <v>124</v>
       </c>
       <c r="T6">
-        <v>28.1</v>
+        <v>30.4</v>
       </c>
       <c r="U6">
+        <v>6.6</v>
+      </c>
+      <c r="V6">
+        <v>6.6</v>
+      </c>
+      <c r="W6">
         <v>6.4</v>
       </c>
-      <c r="V6">
-        <v>6.4</v>
-      </c>
-      <c r="W6">
+      <c r="X6">
+        <v>6.1</v>
+      </c>
+      <c r="Y6">
+        <v>7.5</v>
+      </c>
+      <c r="Z6">
         <v>5.9</v>
-      </c>
-      <c r="X6">
-        <v>6.3</v>
-      </c>
-      <c r="Y6">
-        <v>7</v>
-      </c>
-      <c r="Z6">
-        <v>6.2</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -1126,17 +1126,17 @@
         </is>
       </c>
       <c r="C7">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D7">
-        <v>445</v>
+        <v>745</v>
       </c>
       <c r="E7">
-        <v>0.276</v>
+        <v>0.206</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -1171,17 +1171,17 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -1198,29 +1198,29 @@
         <v>20</v>
       </c>
       <c r="S7">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="T7">
-        <v>36.1</v>
+        <v>44.5</v>
       </c>
       <c r="U7">
+        <v>6.6</v>
+      </c>
+      <c r="V7">
+        <v>6.6</v>
+      </c>
+      <c r="W7">
         <v>6.4</v>
       </c>
-      <c r="V7">
-        <v>6.4</v>
-      </c>
-      <c r="W7">
+      <c r="X7">
+        <v>6.1</v>
+      </c>
+      <c r="Y7">
+        <v>7.5</v>
+      </c>
+      <c r="Z7">
         <v>5.9</v>
       </c>
-      <c r="X7">
-        <v>6.3</v>
-      </c>
-      <c r="Y7">
-        <v>7</v>
-      </c>
-      <c r="Z7">
-        <v>6.2</v>
-      </c>
       <c r="AA7">
         <v>0</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="AD7">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="8">
@@ -1246,17 +1246,17 @@
         </is>
       </c>
       <c r="C8">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D8">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>0.008999999999999999</v>
+        <v>0.007</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -1266,17 +1266,17 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -1315,37 +1315,37 @@
         </is>
       </c>
       <c r="R8">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="S8">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="T8">
-        <v>29.8</v>
+        <v>31.3</v>
       </c>
       <c r="U8">
+        <v>6.6</v>
+      </c>
+      <c r="V8">
+        <v>6.6</v>
+      </c>
+      <c r="W8">
         <v>6.4</v>
       </c>
-      <c r="V8">
-        <v>6.4</v>
-      </c>
-      <c r="W8">
+      <c r="X8">
+        <v>6.1</v>
+      </c>
+      <c r="Y8">
+        <v>7.5</v>
+      </c>
+      <c r="Z8">
         <v>5.9</v>
       </c>
-      <c r="X8">
-        <v>6.3</v>
-      </c>
-      <c r="Y8">
-        <v>7</v>
-      </c>
-      <c r="Z8">
-        <v>6.2</v>
-      </c>
       <c r="AA8">
         <v>0</v>
       </c>
       <c r="AB8">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AC8">
         <v>0</v>
@@ -1366,17 +1366,17 @@
         </is>
       </c>
       <c r="C9">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D9">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="E9">
-        <v>0.012</v>
+        <v>0.02</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -1435,32 +1435,32 @@
         </is>
       </c>
       <c r="R9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S9">
-        <v>129</v>
+        <v>141.5</v>
       </c>
       <c r="T9">
-        <v>30.5</v>
+        <v>49.7</v>
       </c>
       <c r="U9">
+        <v>6.6</v>
+      </c>
+      <c r="V9">
+        <v>6.6</v>
+      </c>
+      <c r="W9">
         <v>6.4</v>
       </c>
-      <c r="V9">
-        <v>6.4</v>
-      </c>
-      <c r="W9">
+      <c r="X9">
+        <v>6.1</v>
+      </c>
+      <c r="Y9">
+        <v>7.5</v>
+      </c>
+      <c r="Z9">
         <v>5.9</v>
       </c>
-      <c r="X9">
-        <v>6.3</v>
-      </c>
-      <c r="Y9">
-        <v>7</v>
-      </c>
-      <c r="Z9">
-        <v>6.2</v>
-      </c>
       <c r="AA9">
         <v>0</v>
       </c>
@@ -1471,47 +1471,47 @@
         <v>0</v>
       </c>
       <c r="AD9">
-        <v>2012</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>3624</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>MBO</t>
         </is>
       </c>
-      <c r="C10">
-        <v>1613</v>
-      </c>
-      <c r="D10">
-        <v>522</v>
-      </c>
-      <c r="E10">
-        <v>0.324</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Direct</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>MBO</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>MedV</t>
+          <t>VS</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1555,64 +1555,64 @@
         </is>
       </c>
       <c r="R10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S10">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="T10">
-        <v>32.7</v>
+        <v>30.4</v>
       </c>
       <c r="U10">
+        <v>6.6</v>
+      </c>
+      <c r="V10">
+        <v>6.6</v>
+      </c>
+      <c r="W10">
         <v>6.4</v>
       </c>
-      <c r="V10">
-        <v>6.4</v>
-      </c>
-      <c r="W10">
+      <c r="X10">
+        <v>6.1</v>
+      </c>
+      <c r="Y10">
+        <v>7.5</v>
+      </c>
+      <c r="Z10">
         <v>5.9</v>
       </c>
-      <c r="X10">
-        <v>6.3</v>
-      </c>
-      <c r="Y10">
-        <v>7</v>
-      </c>
-      <c r="Z10">
-        <v>6.2</v>
-      </c>
       <c r="AA10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AC10">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AD10">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Vooropleiding</t>
+          <t>Aansluiting</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="C11">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D11">
-        <v>860</v>
+        <v>3</v>
       </c>
       <c r="E11">
-        <v>0.533</v>
+        <v>0.001</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1621,12 +1621,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Direct</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>HAVO</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1636,32 +1636,32 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1675,34 +1675,34 @@
         </is>
       </c>
       <c r="R11">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S11">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="T11">
-        <v>35.9</v>
+        <v>44.5</v>
       </c>
       <c r="U11">
+        <v>6.6</v>
+      </c>
+      <c r="V11">
+        <v>6.6</v>
+      </c>
+      <c r="W11">
         <v>6.4</v>
       </c>
-      <c r="V11">
-        <v>6.4</v>
-      </c>
-      <c r="W11">
+      <c r="X11">
+        <v>6.1</v>
+      </c>
+      <c r="Y11">
+        <v>7.5</v>
+      </c>
+      <c r="Z11">
         <v>5.9</v>
       </c>
-      <c r="X11">
-        <v>6.3</v>
-      </c>
-      <c r="Y11">
-        <v>7</v>
-      </c>
-      <c r="Z11">
-        <v>6.2</v>
-      </c>
       <c r="AA11">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -1711,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="AD11">
-        <v>2016</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="12">
@@ -1722,36 +1722,36 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>VWO</t>
+          <t>MBO</t>
         </is>
       </c>
       <c r="C12">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D12">
-        <v>58</v>
+        <v>534</v>
       </c>
       <c r="E12">
-        <v>0.036</v>
+        <v>0.147</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>VWO</t>
+          <t>MBO</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>EA</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1761,27 +1761,27 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1795,34 +1795,34 @@
         </is>
       </c>
       <c r="R12">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="S12">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="T12">
-        <v>30.9</v>
+        <v>38.4</v>
       </c>
       <c r="U12">
+        <v>6.6</v>
+      </c>
+      <c r="V12">
+        <v>6.6</v>
+      </c>
+      <c r="W12">
         <v>6.4</v>
       </c>
-      <c r="V12">
-        <v>6.4</v>
-      </c>
-      <c r="W12">
+      <c r="X12">
+        <v>6.1</v>
+      </c>
+      <c r="Y12">
+        <v>7.5</v>
+      </c>
+      <c r="Z12">
         <v>5.9</v>
       </c>
-      <c r="X12">
-        <v>6.3</v>
-      </c>
-      <c r="Y12">
-        <v>7</v>
-      </c>
-      <c r="Z12">
-        <v>6.2</v>
-      </c>
       <c r="AA12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="AB12">
         <v>0</v>
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="AD12">
-        <v>2016</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="13">
@@ -1842,21 +1842,21 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BD</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="C13">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D13">
-        <v>92</v>
+        <v>1880</v>
       </c>
       <c r="E13">
-        <v>0.057</v>
+        <v>0.519</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1866,42 +1866,42 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>BD</t>
+          <t>HAVO</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Onbekend</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1915,37 +1915,37 @@
         </is>
       </c>
       <c r="R13">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="S13">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="T13">
-        <v>15.5</v>
+        <v>45.9</v>
       </c>
       <c r="U13">
+        <v>6.6</v>
+      </c>
+      <c r="V13">
+        <v>6.6</v>
+      </c>
+      <c r="W13">
         <v>6.4</v>
       </c>
-      <c r="V13">
-        <v>6.4</v>
-      </c>
-      <c r="W13">
+      <c r="X13">
+        <v>6.1</v>
+      </c>
+      <c r="Y13">
+        <v>7.5</v>
+      </c>
+      <c r="Z13">
         <v>5.9</v>
       </c>
-      <c r="X13">
-        <v>6.3</v>
-      </c>
-      <c r="Y13">
-        <v>7</v>
-      </c>
-      <c r="Z13">
-        <v>6.2</v>
-      </c>
       <c r="AA13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB13">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AC13">
         <v>0</v>
@@ -1962,36 +1962,36 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>VWO</t>
         </is>
       </c>
       <c r="C14">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D14">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="E14">
-        <v>0.019</v>
+        <v>0.016</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>V</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Na CD</t>
+          <t>Switch extern</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>CD</t>
+          <t>VWO</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>EM</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -2001,27 +2001,27 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Ja</t>
+          <t>Nee</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -2035,43 +2035,43 @@
         </is>
       </c>
       <c r="R14">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="S14">
-        <v>127.5</v>
+        <v>141</v>
       </c>
       <c r="T14">
-        <v>29.6</v>
+        <v>39.8</v>
       </c>
       <c r="U14">
+        <v>6.6</v>
+      </c>
+      <c r="V14">
+        <v>6.6</v>
+      </c>
+      <c r="W14">
         <v>6.4</v>
       </c>
-      <c r="V14">
-        <v>6.4</v>
-      </c>
-      <c r="W14">
+      <c r="X14">
+        <v>6.1</v>
+      </c>
+      <c r="Y14">
+        <v>7.5</v>
+      </c>
+      <c r="Z14">
         <v>5.9</v>
       </c>
-      <c r="X14">
-        <v>6.3</v>
-      </c>
-      <c r="Y14">
-        <v>7</v>
-      </c>
-      <c r="Z14">
-        <v>6.2</v>
-      </c>
       <c r="AA14">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="AB14">
-        <v>-0</v>
+        <v>0.1</v>
       </c>
       <c r="AC14">
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>2017.5</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="15">
@@ -2082,17 +2082,17 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>HO</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="C15">
-        <v>1613</v>
+        <v>3624</v>
       </c>
       <c r="D15">
-        <v>51</v>
+        <v>1031</v>
       </c>
       <c r="E15">
-        <v>0.032</v>
+        <v>0.284</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2101,12 +2101,12 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Switch extern</t>
+          <t>Direct</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>HO</t>
+          <t>BD</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -2116,32 +2116,32 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Onbekend</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Nee</t>
+          <t>Ja</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
@@ -2158,40 +2158,400 @@
         <v>20</v>
       </c>
       <c r="S15">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="T15">
-        <v>38.3</v>
+        <v>31.9</v>
       </c>
       <c r="U15">
+        <v>6.6</v>
+      </c>
+      <c r="V15">
+        <v>6.6</v>
+      </c>
+      <c r="W15">
         <v>6.4</v>
       </c>
-      <c r="V15">
+      <c r="X15">
+        <v>6.1</v>
+      </c>
+      <c r="Y15">
+        <v>7.5</v>
+      </c>
+      <c r="Z15">
+        <v>5.9</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Vooropleiding</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>3624</v>
+      </c>
+      <c r="D16">
+        <v>82</v>
+      </c>
+      <c r="E16">
+        <v>0.023</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Na CD</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>CD</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>EM</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="R16">
+        <v>21</v>
+      </c>
+      <c r="S16">
+        <v>141.5</v>
+      </c>
+      <c r="T16">
+        <v>49.7</v>
+      </c>
+      <c r="U16">
+        <v>6.6</v>
+      </c>
+      <c r="V16">
+        <v>6.6</v>
+      </c>
+      <c r="W16">
         <v>6.4</v>
       </c>
-      <c r="W15">
+      <c r="X16">
+        <v>6.1</v>
+      </c>
+      <c r="Y16">
+        <v>7.5</v>
+      </c>
+      <c r="Z16">
         <v>5.9</v>
       </c>
-      <c r="X15">
-        <v>6.3</v>
-      </c>
-      <c r="Y15">
-        <v>7</v>
-      </c>
-      <c r="Z15">
-        <v>6.2</v>
-      </c>
-      <c r="AA15">
-        <v>0.1</v>
-      </c>
-      <c r="AB15">
-        <v>0.1</v>
-      </c>
-      <c r="AC15">
-        <v>0</v>
-      </c>
-      <c r="AD15">
-        <v>2015</v>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>2016.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Vooropleiding</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>HO</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>3624</v>
+      </c>
+      <c r="D17">
+        <v>23</v>
+      </c>
+      <c r="E17">
+        <v>0.006</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Switch extern</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>HO</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>EM</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="R17">
+        <v>19</v>
+      </c>
+      <c r="S17">
+        <v>133</v>
+      </c>
+      <c r="T17">
+        <v>44.5</v>
+      </c>
+      <c r="U17">
+        <v>6.6</v>
+      </c>
+      <c r="V17">
+        <v>6.6</v>
+      </c>
+      <c r="W17">
+        <v>6.4</v>
+      </c>
+      <c r="X17">
+        <v>6.1</v>
+      </c>
+      <c r="Y17">
+        <v>7.5</v>
+      </c>
+      <c r="Z17">
+        <v>5.9</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Vooropleiding</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>3624</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>0.004</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Direct</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Overig</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>EM</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Onbekend</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>Ja</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>Nee</t>
+        </is>
+      </c>
+      <c r="R18">
+        <v>19</v>
+      </c>
+      <c r="S18">
+        <v>125</v>
+      </c>
+      <c r="T18">
+        <v>44.5</v>
+      </c>
+      <c r="U18">
+        <v>6.6</v>
+      </c>
+      <c r="V18">
+        <v>6.6</v>
+      </c>
+      <c r="W18">
+        <v>6.4</v>
+      </c>
+      <c r="X18">
+        <v>6.1</v>
+      </c>
+      <c r="Y18">
+        <v>7.5</v>
+      </c>
+      <c r="Z18">
+        <v>5.9</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>